<commit_message>
renamed label of size attribute in Product_Size to Size
</commit_message>
<xml_diff>
--- a/legacy/clean/size.xlsx
+++ b/legacy/clean/size.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Product Size</t>
+          <t>Size</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2021-02-03</t>
+          <t>2021-02-04</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2021-02-03</t>
+          <t>2021-02-04</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2021-02-03</t>
+          <t>2021-02-04</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2021-02-03</t>
+          <t>2021-02-04</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2021-02-03</t>
+          <t>2021-02-04</t>
         </is>
       </c>
     </row>
@@ -548,7 +548,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2021-02-03</t>
+          <t>2021-02-04</t>
         </is>
       </c>
     </row>

</xml_diff>